<commit_message>
Trabajando en datos Tutores
</commit_message>
<xml_diff>
--- a/extras/datos/Lista Turorias 2019 luis.csv.xlsx
+++ b/extras/datos/Lista Turorias 2019 luis.csv.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="439">
   <si>
     <t>APELLIDO PATERNO</t>
   </si>
@@ -732,9 +733,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>9713483929</t>
-  </si>
-  <si>
     <t>9713978343</t>
   </si>
   <si>
@@ -922,6 +920,429 @@
   </si>
   <si>
     <t>/directory/img-person/MagdaGuadalupeToledo.jpg</t>
+  </si>
+  <si>
+    <t>ARAGON</t>
+  </si>
+  <si>
+    <t>REYES</t>
+  </si>
+  <si>
+    <t>VERA ALEXANDRO</t>
+  </si>
+  <si>
+    <t>PERALTA</t>
+  </si>
+  <si>
+    <t>GONZALEZ</t>
+  </si>
+  <si>
+    <t>LORENA</t>
+  </si>
+  <si>
+    <t>MEDINA</t>
+  </si>
+  <si>
+    <t>ALEGRIA</t>
+  </si>
+  <si>
+    <t>LEONEL ADELFO</t>
+  </si>
+  <si>
+    <t>UICAB</t>
+  </si>
+  <si>
+    <t>AYALA</t>
+  </si>
+  <si>
+    <t>BIENVENIDO ANGEL</t>
+  </si>
+  <si>
+    <t>OROZCO</t>
+  </si>
+  <si>
+    <t>ALVAREZ</t>
+  </si>
+  <si>
+    <t>SAYONARA</t>
+  </si>
+  <si>
+    <t>NOLASCO</t>
+  </si>
+  <si>
+    <t>VERONICA</t>
+  </si>
+  <si>
+    <t>LOPEZ</t>
+  </si>
+  <si>
+    <t>ALBINO</t>
+  </si>
+  <si>
+    <t>GOMEZ</t>
+  </si>
+  <si>
+    <t>PINEDA</t>
+  </si>
+  <si>
+    <t>GICELA ALICIA</t>
+  </si>
+  <si>
+    <t>GUERRA</t>
+  </si>
+  <si>
+    <t>IRMA FLOR</t>
+  </si>
+  <si>
+    <t>NUÑEZ</t>
+  </si>
+  <si>
+    <t>MARIA DEL ROSARIO</t>
+  </si>
+  <si>
+    <t>PERALES</t>
+  </si>
+  <si>
+    <t>JOSE FELICIANO</t>
+  </si>
+  <si>
+    <t>CASTILLEJOS</t>
+  </si>
+  <si>
+    <t>TOLEDO</t>
+  </si>
+  <si>
+    <t>MARIBEL</t>
+  </si>
+  <si>
+    <t>ECHEVERRIA</t>
+  </si>
+  <si>
+    <t>ORTIZ</t>
+  </si>
+  <si>
+    <t>JAVIER EDUARDO</t>
+  </si>
+  <si>
+    <t>CRUZ</t>
+  </si>
+  <si>
+    <t>LUCIANO</t>
+  </si>
+  <si>
+    <t>DEHESA</t>
+  </si>
+  <si>
+    <t>VALENCIA</t>
+  </si>
+  <si>
+    <t>GASTON</t>
+  </si>
+  <si>
+    <t>JOSE MANUEL</t>
+  </si>
+  <si>
+    <t>MARANTO</t>
+  </si>
+  <si>
+    <t>IGLECIAS</t>
+  </si>
+  <si>
+    <t>JORGE</t>
+  </si>
+  <si>
+    <t>RASGADO</t>
+  </si>
+  <si>
+    <t>SANCHEZ</t>
+  </si>
+  <si>
+    <t>JUVENAL</t>
+  </si>
+  <si>
+    <t>BLAS</t>
+  </si>
+  <si>
+    <t>MARIANO</t>
+  </si>
+  <si>
+    <t>POSADA</t>
+  </si>
+  <si>
+    <t>JOSE ANTONIO</t>
+  </si>
+  <si>
+    <t>CHIRINOS</t>
+  </si>
+  <si>
+    <t>JESUS</t>
+  </si>
+  <si>
+    <t>ALEIDA</t>
+  </si>
+  <si>
+    <t>CORDOVA</t>
+  </si>
+  <si>
+    <t>MARIO</t>
+  </si>
+  <si>
+    <t>VALDIVIESO</t>
+  </si>
+  <si>
+    <t>MARIA ISABEL</t>
+  </si>
+  <si>
+    <t>OLIVARES</t>
+  </si>
+  <si>
+    <t>PEREZ</t>
+  </si>
+  <si>
+    <t>ANGEL</t>
+  </si>
+  <si>
+    <t>QUIÑONES</t>
+  </si>
+  <si>
+    <t>IRMA</t>
+  </si>
+  <si>
+    <t>RUIZ</t>
+  </si>
+  <si>
+    <t>IVAN</t>
+  </si>
+  <si>
+    <t>CELAYA</t>
+  </si>
+  <si>
+    <t>FLAVIO AQUILES</t>
+  </si>
+  <si>
+    <t>RAMIREZ</t>
+  </si>
+  <si>
+    <t>REGALADO</t>
+  </si>
+  <si>
+    <t>ALBERTO</t>
+  </si>
+  <si>
+    <t>GARCIA</t>
+  </si>
+  <si>
+    <t>DANIEL</t>
+  </si>
+  <si>
+    <t>VARELA</t>
+  </si>
+  <si>
+    <t>RUBEN</t>
+  </si>
+  <si>
+    <t>RIVERA</t>
+  </si>
+  <si>
+    <t>CASTILLO</t>
+  </si>
+  <si>
+    <t>RANULFO</t>
+  </si>
+  <si>
+    <t>direccion de prueba</t>
+  </si>
+  <si>
+    <t>9718920270</t>
+  </si>
+  <si>
+    <t>9719384559</t>
+  </si>
+  <si>
+    <t>9714692850</t>
+  </si>
+  <si>
+    <t>9716470322</t>
+  </si>
+  <si>
+    <t>9711671138</t>
+  </si>
+  <si>
+    <t>9719199594</t>
+  </si>
+  <si>
+    <t>9714472540</t>
+  </si>
+  <si>
+    <t>9717024457</t>
+  </si>
+  <si>
+    <t>9713287678</t>
+  </si>
+  <si>
+    <t>9718557052</t>
+  </si>
+  <si>
+    <t>9716187488</t>
+  </si>
+  <si>
+    <t>9712378043</t>
+  </si>
+  <si>
+    <t>9716397301</t>
+  </si>
+  <si>
+    <t>9714904778</t>
+  </si>
+  <si>
+    <t>9714183592</t>
+  </si>
+  <si>
+    <t>9714704422</t>
+  </si>
+  <si>
+    <t>9719707889</t>
+  </si>
+  <si>
+    <t>9711701459</t>
+  </si>
+  <si>
+    <t>9711902494</t>
+  </si>
+  <si>
+    <t>9717607379</t>
+  </si>
+  <si>
+    <t>9715715806</t>
+  </si>
+  <si>
+    <t>9713945180</t>
+  </si>
+  <si>
+    <t>9711885289</t>
+  </si>
+  <si>
+    <t>9716011990</t>
+  </si>
+  <si>
+    <t>9716192621</t>
+  </si>
+  <si>
+    <t>9718683195</t>
+  </si>
+  <si>
+    <t>9719497746</t>
+  </si>
+  <si>
+    <t>9715067184</t>
+  </si>
+  <si>
+    <t>9718583372</t>
+  </si>
+  <si>
+    <t>9716232169</t>
+  </si>
+  <si>
+    <t>9719987378</t>
+  </si>
+  <si>
+    <t>9712325600</t>
+  </si>
+  <si>
+    <t>/directory/img-person/LORENAGONZALEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/SAYONARAALVAREZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/VERONICANOLASCO.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/ALBINOLOPEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/MARIBELTOLEDO.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/LUCIANOCRUZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/GASTONVALENCIA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JORGEIGLECIAS.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JUVENALSANCHEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/MARIANOSANCHEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JESUSCHIRINOS.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/ALEIDASANCHEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/MARIOCORDOVA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/ANGELPEREZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/IRMAPINEDA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/IVANSANCHEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/ALBERTOREGALADO.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/DANIELOROZCO.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/RUBENVARELA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/RANULFOCASTILLO.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/LEONELADELFOALEGRIA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/BIENVENIDOANGELAYALA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/GICELAALICIAPINEDA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/IRMAFLORGUERRA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/MARIADELROSARIOLOPEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JOSEFELICIANOPERALES.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JAVIEREDUARDOORTIZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JOSEMANUELGONZALEZ.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/JOSEANTONIOPOSADA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/MARIAISABELVALDIVIESO.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/FLAVIOAQUILESCELAYA.jpg</t>
+  </si>
+  <si>
+    <t>/directory/img-person/VERAALEXANDROREYES.jpg</t>
   </si>
 </sst>
 </file>
@@ -966,7 +1387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -977,6 +1398,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -3193,8 +3615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="G1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3239,10 +3661,10 @@
         <v>232</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3265,23 +3687,23 @@
         <f>CONCATENATE(B2,A2,LEFT(C2,2),"@gmail.com")</f>
         <v>JiménezToledoMa@gmail.com</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>235</v>
+      <c r="G2" s="1">
+        <v>9713483929</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M2">
         <f>COUNTIF(E:E,"M")</f>
@@ -3309,22 +3731,22 @@
         <v>PastelinToledoDa@gmail.com</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M3">
         <f>COUNTIF(E:E,"F")</f>
@@ -3352,19 +3774,19 @@
         <v>HernandezToralMa@gmail.com</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" t="s">
+        <v>284</v>
+      </c>
+      <c r="K4" t="s">
         <v>264</v>
-      </c>
-      <c r="J4" t="s">
-        <v>285</v>
-      </c>
-      <c r="K4" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -3388,19 +3810,19 @@
         <v>MoralesToralJo@gmail.com</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -3424,19 +3846,19 @@
         <v>JiménezTrujilloCa@gmail.com</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -3460,19 +3882,19 @@
         <v>AlvarezNoriegaDa@gmail.com</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -3496,19 +3918,19 @@
         <v>FuentesOlivarezDa@gmail.com</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -3532,19 +3954,19 @@
         <v>MoralesOrdazDa@gmail.com</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -3568,16 +3990,16 @@
         <v>OrozcoOrdazMa@gmail.com</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -3601,16 +4023,16 @@
         <v>LopezPalomecJo@gmail.com</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -3634,16 +4056,16 @@
         <v>MartínezPerezPe@gmail.com</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -3667,16 +4089,16 @@
         <v>LugoRamírezEl@gmail.com</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -3700,16 +4122,16 @@
         <v>JoseRamosSe@gmail.com</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -3733,16 +4155,16 @@
         <v>LópezRasgadoCa@gmail.com</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -3766,16 +4188,16 @@
         <v>NuñezRuízll@gmail.com</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3799,16 +4221,16 @@
         <v>SánchezRuízAr@gmail.com</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3832,16 +4254,16 @@
         <v>ToledoJiménezEs@gmail.com</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3865,16 +4287,16 @@
         <v>GarcíaLaureanoLu@gmail.com</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3898,16 +4320,16 @@
         <v>HernandezLópezEd@gmail.com</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3931,16 +4353,16 @@
         <v>LópezLópezKe@gmail.com</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3964,16 +4386,16 @@
         <v>LópezLópezRe@gmail.com</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3997,16 +4419,16 @@
         <v>MatusLópezVl@gmail.com</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -4030,16 +4452,16 @@
         <v>ChicatyMartínezPa@gmail.com</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -4063,16 +4485,16 @@
         <v>MartínezMatusGu@gmail.com</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -4096,17 +4518,1200 @@
         <v>OrdazMatusJo@gmail.com</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>259</v>
       </c>
+      <c r="I26" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J26" t="s">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="51.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" s="2">
+        <v>30920</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F2" s="3" t="str">
+        <f>CONCATENATE(B2,A2,LEFT(C2,2),"@gmail.com")</f>
+        <v>REYESARAGONVE@gmail.com</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J2" t="s">
+        <v>438</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIF(E:E,"M")</f>
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D3" s="2">
+        <v>22900</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <f t="shared" ref="F3:F33" si="0">CONCATENATE(B3,A3,LEFT(C3,2),"@gmail.com")</f>
+        <v>GONZALEZPERALTALO@gmail.com</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J3" t="s">
+        <v>407</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L3">
+        <f>COUNTIF(E:E,"F")</f>
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D4" s="2">
+        <v>26063</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ALEGRIAMEDINALE@gmail.com</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J4" t="s">
+        <v>427</v>
+      </c>
+      <c r="N4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" s="2">
+        <v>29610</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>AYALAUICABBI@gmail.com</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J5" t="s">
+        <v>428</v>
+      </c>
+      <c r="N5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D6" s="2">
+        <v>28418</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ALVAREZOROZCOSA@gmail.com</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J6" t="s">
+        <v>408</v>
+      </c>
+      <c r="N6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D7" s="2">
+        <v>33208</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>NOLASCOOROZCOVE@gmail.com</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J7" t="s">
+        <v>409</v>
+      </c>
+      <c r="N7" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" s="2">
+        <v>22670</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>LOPEZLOPEZAL@gmail.com</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J8" t="s">
+        <v>410</v>
+      </c>
+      <c r="N8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="2">
+        <v>25277</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PINEDAGOMEZGI@gmail.com</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J9" t="s">
+        <v>429</v>
+      </c>
+      <c r="N9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="2">
+        <v>26704</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>GUERRALOPEZIR@gmail.com</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J10" t="s">
+        <v>430</v>
+      </c>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D11" s="2">
+        <v>25769</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>LOPEZNUÑEZMA@gmail.com</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J11" t="s">
+        <v>431</v>
+      </c>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D12" s="2">
+        <v>25337</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PERALESLOPEZJO@gmail.com</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J12" t="s">
+        <v>432</v>
+      </c>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D13" s="2">
+        <v>27587</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>TOLEDOCASTILLEJOSMA@gmail.com</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J13" t="s">
+        <v>411</v>
+      </c>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D14" s="2">
+        <v>22190</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>ORTIZECHEVERRIAJA@gmail.com</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J14" t="s">
+        <v>433</v>
+      </c>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="D15" s="2">
+        <v>28224</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CRUZTOLEDOLU@gmail.com</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J15" t="s">
+        <v>412</v>
+      </c>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D16" s="2">
+        <v>29771</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>VALENCIADEHESAGA@gmail.com</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J16" t="s">
+        <v>413</v>
+      </c>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D17" s="2">
+        <v>29744</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>GONZALEZCASTILLEJOSJO@gmail.com</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J17" t="s">
+        <v>434</v>
+      </c>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D18" s="2">
+        <v>25110</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>IGLECIASMARANTOJO@gmail.com</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J18" t="s">
+        <v>414</v>
+      </c>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D19" s="2">
+        <v>25233</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SANCHEZRASGADOJU@gmail.com</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J19" t="s">
+        <v>415</v>
+      </c>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="D20" s="2">
+        <v>30857</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SANCHEZBLASMA@gmail.com</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J20" t="s">
+        <v>416</v>
+      </c>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D21" s="2">
+        <v>22537</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>POSADALOPEZJO@gmail.com</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J21" t="s">
+        <v>435</v>
+      </c>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="D22" s="2">
+        <v>28700</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CHIRINOSLOPEZJE@gmail.com</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J22" t="s">
+        <v>417</v>
+      </c>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="D23" s="2">
+        <v>30593</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SANCHEZOROZCOAL@gmail.com</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="J23" t="s">
+        <v>418</v>
+      </c>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D24" s="2">
+        <v>25544</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CORDOVANUÑEZMA@gmail.com</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J24" t="s">
+        <v>419</v>
+      </c>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D25" s="2">
+        <v>25121</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>VALDIVIESOGOMEZMA@gmail.com</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J25" t="s">
+        <v>436</v>
+      </c>
+      <c r="N25" s="4"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D26" s="2">
+        <v>29515</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PEREZOLIVARESAN@gmail.com</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>399</v>
+      </c>
       <c r="H26" s="1" t="s">
-        <v>260</v>
+        <v>374</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J26" t="s">
-        <v>297</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D27" s="2">
+        <v>24592</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PINEDAQUIÑONESIR@gmail.com</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="J27" t="s">
+        <v>421</v>
+      </c>
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D28" s="2">
+        <v>32627</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>SANCHEZRUIZIV@gmail.com</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J28" t="s">
+        <v>422</v>
+      </c>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D29" s="2">
+        <v>27871</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CELAYARUIZFL@gmail.com</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="J29" t="s">
+        <v>437</v>
+      </c>
+      <c r="N29" s="4"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D30" s="2">
+        <v>29515</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>REGALADORAMIREZAL@gmail.com</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J30" t="s">
+        <v>423</v>
+      </c>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D31" s="2">
+        <v>23719</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>OROZCOGARCIADA@gmail.com</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="J31" t="s">
+        <v>424</v>
+      </c>
+      <c r="N31" s="4"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D32" s="2">
+        <v>30772</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>VARELAMEDINARU@gmail.com</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J32" t="s">
+        <v>425</v>
+      </c>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D33" s="2">
+        <v>27662</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CASTILLORIVERARA@gmail.com</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="J33" t="s">
+        <v>426</v>
+      </c>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D34" s="4"/>
+      <c r="N34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
anexando datos de profesores
</commit_message>
<xml_diff>
--- a/extras/datos/Lista Turorias 2019 luis.csv.xlsx
+++ b/extras/datos/Lista Turorias 2019 luis.csv.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tutorias\extras\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D909A8-B899-46AE-AF99-8C5DD9AFA543}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="444">
   <si>
     <t>APELLIDO PATERNO</t>
   </si>
@@ -1346,12 +1353,24 @@
   </si>
   <si>
     <t>"</t>
+  </si>
+  <si>
+    <t>JIMÉNEZ</t>
+  </si>
+  <si>
+    <t>VICTOR MANUEL</t>
+  </si>
+  <si>
+    <t>9715765171</t>
+  </si>
+  <si>
+    <t>/directory/img-person/VICTORMANUELJIMENEZ.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1442,7 +1461,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="2"/>
       <tableStyleElement type="headerRow" dxfId="1"/>
     </tableStyle>
@@ -1720,23 +1739,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1753,7 +1772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1770,7 +1789,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1787,7 +1806,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1804,7 +1823,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1821,7 +1840,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1838,7 +1857,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1855,7 +1874,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1872,7 +1891,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1889,7 +1908,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1906,7 +1925,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1923,7 +1942,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1940,7 +1959,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -1957,7 +1976,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1974,7 +1993,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1991,7 +2010,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2008,7 +2027,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2025,7 +2044,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2042,7 +2061,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2059,7 +2078,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2076,7 +2095,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2093,7 +2112,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2110,7 +2129,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2127,7 +2146,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2144,7 +2163,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2161,7 +2180,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2178,7 +2197,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2195,7 +2214,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2212,7 +2231,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -2229,7 +2248,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2246,7 +2265,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2263,7 +2282,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2280,7 +2299,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2297,7 +2316,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2314,7 +2333,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2331,7 +2350,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2348,7 +2367,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2365,7 +2384,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2382,7 +2401,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -2399,7 +2418,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>93</v>
       </c>
@@ -2416,7 +2435,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -2433,7 +2452,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2450,7 +2469,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>105</v>
       </c>
@@ -2467,7 +2486,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -2484,7 +2503,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -2501,7 +2520,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>109</v>
       </c>
@@ -2518,7 +2537,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>111</v>
       </c>
@@ -2535,7 +2554,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -2552,7 +2571,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>114</v>
       </c>
@@ -2569,7 +2588,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2586,7 +2605,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -2603,7 +2622,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>125</v>
       </c>
@@ -2620,7 +2639,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>127</v>
       </c>
@@ -2637,7 +2656,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>129</v>
       </c>
@@ -2654,7 +2673,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>129</v>
       </c>
@@ -2671,7 +2690,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>129</v>
       </c>
@@ -2688,7 +2707,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>132</v>
       </c>
@@ -2705,7 +2724,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -2722,7 +2741,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -2739,7 +2758,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -2756,7 +2775,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -2773,7 +2792,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -2790,7 +2809,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>145</v>
       </c>
@@ -2807,7 +2826,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -2824,7 +2843,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>146</v>
       </c>
@@ -2841,7 +2860,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -2858,7 +2877,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2875,7 +2894,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2892,7 +2911,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -2909,7 +2928,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -2926,7 +2945,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -2943,7 +2962,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>158</v>
       </c>
@@ -2960,7 +2979,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -2977,7 +2996,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>106</v>
       </c>
@@ -2994,7 +3013,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>160</v>
       </c>
@@ -3011,7 +3030,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>162</v>
       </c>
@@ -3028,7 +3047,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>95</v>
       </c>
@@ -3045,7 +3064,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>168</v>
       </c>
@@ -3062,7 +3081,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>170</v>
       </c>
@@ -3079,7 +3098,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -3096,7 +3115,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>172</v>
       </c>
@@ -3113,7 +3132,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>173</v>
       </c>
@@ -3130,7 +3149,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -3147,7 +3166,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>184</v>
       </c>
@@ -3164,7 +3183,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>186</v>
       </c>
@@ -3181,7 +3200,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>187</v>
       </c>
@@ -3198,7 +3217,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -3215,7 +3234,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>169</v>
       </c>
@@ -3232,7 +3251,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>189</v>
       </c>
@@ -3249,7 +3268,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>191</v>
       </c>
@@ -3266,7 +3285,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -3283,7 +3302,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>200</v>
       </c>
@@ -3300,7 +3319,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>26</v>
       </c>
@@ -3317,7 +3336,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>26</v>
       </c>
@@ -3334,7 +3353,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>145</v>
       </c>
@@ -3351,7 +3370,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>30</v>
       </c>
@@ -3368,7 +3387,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>30</v>
       </c>
@@ -3385,7 +3404,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>46</v>
       </c>
@@ -3402,7 +3421,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>46</v>
       </c>
@@ -3419,7 +3438,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>46</v>
       </c>
@@ -3436,7 +3455,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>162</v>
       </c>
@@ -3453,7 +3472,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>209</v>
       </c>
@@ -3470,7 +3489,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>208</v>
       </c>
@@ -3487,7 +3506,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>217</v>
       </c>
@@ -3504,7 +3523,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>5</v>
       </c>
@@ -3521,7 +3540,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>73</v>
       </c>
@@ -3538,7 +3557,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>219</v>
       </c>
@@ -3555,7 +3574,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>220</v>
       </c>
@@ -3572,7 +3591,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>222</v>
       </c>
@@ -3589,7 +3608,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>223</v>
       </c>
@@ -3615,32 +3634,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScale="82" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" customWidth="1"/>
-    <col min="10" max="10" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="30.5546875" customWidth="1"/>
+    <col min="10" max="10" width="56.109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="218" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3672,7 +3691,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3719,7 +3738,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -3766,7 +3785,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3806,7 +3825,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3846,7 +3865,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -3886,7 +3905,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -3926,7 +3945,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -3966,7 +3985,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -4006,7 +4025,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -4046,7 +4065,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -4083,7 +4102,7 @@
         <v>INSERT INTO 'persona' VALUES ("Jorge Antonio","Palomec","Lopez",08/11/1998,"M","LopezPalomecJo@gmail.com","9712152501","direccion prueba","Tehuantepec","/directory/img-person/JorgeAntonioPalomec.jpg"</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -4120,7 +4139,7 @@
         <v>INSERT INTO 'persona' VALUES ("Pedro Alberto","Perez","Martínez",14/03/1999,"M","MartínezPerezPe@gmail.com","9715094524","direccion prueba","Ixtepec","/directory/img-person/PedroAlbertoPerez.jpg"</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -4157,7 +4176,7 @@
         <v>INSERT INTO 'persona' VALUES ("Elías","Ramírez","Lugo",12/05/1999,"M","LugoRamírezEl@gmail.com","9716779058","direccion prueba","Juchitán","/directory/img-person/ElíasRamírez.jpg"</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -4194,7 +4213,7 @@
         <v>INSERT INTO 'persona' VALUES ("Sergio Manuel","Ramos","Jose",17/01/1999,"M","JoseRamosSe@gmail.com","9718404624","direccion prueba","Juchitán","/directory/img-person/SergioManuelRamos.jpg"</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -4231,7 +4250,7 @@
         <v>INSERT INTO 'persona' VALUES ("Carlos","Rasgado","López",18/08/1999,"M","LópezRasgadoCa@gmail.com","9718326392","direccion prueba","Chicapa","/directory/img-person/CarlosRasgado.jpg"</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -4268,7 +4287,7 @@
         <v>INSERT INTO 'persona' VALUES ("llliane Monserrat","Ruíz","Nuñez",20/09/1999,"F","NuñezRuízll@gmail.com","9713854313","direccion prueba","Salina Cruz","/directory/img-person/lllianeMonserratRuíz.jpg"</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -4305,7 +4324,7 @@
         <v>INSERT INTO 'persona' VALUES ("Arnulfo","Ruíz","Sánchez",17/06/1999,"M","SánchezRuízAr@gmail.com","9712820548","direccion prueba","Espinal","/directory/img-person/ArnulfoRuíz.jpg"</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -4342,7 +4361,7 @@
         <v>INSERT INTO 'persona' VALUES ("Esmeralda Yolotzin","Jiménez","Toledo",28/04/1999,"F","ToledoJiménezEs@gmail.com","9711441871","direccion prueba","Unión Hidalgo","/directory/img-person/EsmeraldaYolotzinJiménez.jpg"</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -4379,7 +4398,7 @@
         <v>INSERT INTO 'persona' VALUES ("Luis Alberto","Laureano","García",17/07/1999,"M","GarcíaLaureanoLu@gmail.com","9714388238","direccion prueba","Salina Cruz","/directory/img-person/LuisAlbertoLaureano.jpg"</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -4416,7 +4435,7 @@
         <v>INSERT INTO 'persona' VALUES ("Edwin","López","Hernandez",08/11/1997,"M","HernandezLópezEd@gmail.com","9715202809","direccion prueba","Unión Hidalgo","/directory/img-person/EdwinLópez.jpg"</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -4453,7 +4472,7 @@
         <v>INSERT INTO 'persona' VALUES ("Kevin","López","López",07/12/1999,"M","LópezLópezKe@gmail.com","9718406718","direccion prueba","Juchitán","/directory/img-person/KevinLópez.jpg"</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -4490,7 +4509,7 @@
         <v>INSERT INTO 'persona' VALUES ("Rey David","López","López",02/11/1999,"M","LópezLópezRe@gmail.com","9715018270","direccion prueba","Ixtepec","/directory/img-person/ReyDavidLópez.jpg"</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -4527,7 +4546,7 @@
         <v>INSERT INTO 'persona' VALUES ("Vladimir Orion","López","Matus",13/08/1997,"M","MatusLópezVl@gmail.com","9712271009","direccion prueba","Unión Hidalgo","/directory/img-person/VladimirOrionLópez.jpg"</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -4564,7 +4583,7 @@
         <v>INSERT INTO 'persona' VALUES ("Patricia Dhamar","Martínez","Chicaty",25/07/1999,"F","ChicatyMartínezPa@gmail.com","9719884435","direccion prueba","Ixtaltepec","/directory/img-person/PatriciaDhamarMartínez.jpg"</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -4601,7 +4620,7 @@
         <v>INSERT INTO 'persona' VALUES ("Guadalupe","Matus","Martínez",16/03/1998,"F","MartínezMatusGu@gmail.com","9714017985","direccion prueba","Espinal","/directory/img-person/GuadalupeMatus.jpg"</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -4644,33 +4663,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="51.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="196.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="51.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="196.33203125" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="19" max="19" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4702,7 +4721,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>298</v>
       </c>
@@ -4743,13 +4762,13 @@
       </c>
       <c r="Q2">
         <f>COUNTIF(E:E,"M")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>301</v>
       </c>
@@ -4766,7 +4785,7 @@
         <v>234</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F33" si="0">CONCATENATE(B3,A3,LEFT(C3,2),"@gmail.com")</f>
+        <f t="shared" ref="F3:F35" si="0">CONCATENATE(B3,A3,LEFT(C3,2),"@gmail.com")</f>
         <v>GONZALEZPERALTALO@gmail.com</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -4782,7 +4801,7 @@
         <v>407</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L33" si="1">CONCATENATE("INSERT INTO 'persona' VALUES (",$S$2,C3,$S$2,",",$S$2,A3,$S$2,",",$S$2,B3,$S$2,",",TEXT(D3,"dd/mm/aaaa"),",",$S$2,E3,$S$2,",",$S$2,F3,$S$2,",",$S$2,G3,$S$2,",",$S$2,H3,$S$2,",",$S$2,I3,$S$2,",",$S$2,J3,$S$2)</f>
+        <f t="shared" ref="L3:L34" si="1">CONCATENATE("INSERT INTO 'persona' VALUES (",$S$2,C3,$S$2,",",$S$2,A3,$S$2,",",$S$2,B3,$S$2,",",TEXT(D3,"dd/mm/aaaa"),",",$S$2,E3,$S$2,",",$S$2,F3,$S$2,",",$S$2,G3,$S$2,",",$S$2,H3,$S$2,",",$S$2,I3,$S$2,",",$S$2,J3,$S$2)</f>
         <v>INSERT INTO 'persona' VALUES ("LORENA","PERALTA","GONZALEZ",11/09/1962,"F","GONZALEZPERALTALO@gmail.com","9719384559","direccion de prueba","Espinal","/directory/img-person/LORENAGONZALEZ.jpg"</v>
       </c>
       <c r="P3" s="1" t="s">
@@ -4796,7 +4815,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>304</v>
       </c>
@@ -4836,7 +4855,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>307</v>
       </c>
@@ -4876,7 +4895,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>310</v>
       </c>
@@ -4916,7 +4935,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>310</v>
       </c>
@@ -4956,7 +4975,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>315</v>
       </c>
@@ -4996,7 +5015,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>317</v>
       </c>
@@ -5036,7 +5055,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>315</v>
       </c>
@@ -5074,7 +5093,7 @@
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>322</v>
       </c>
@@ -5112,7 +5131,7 @@
       </c>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>315</v>
       </c>
@@ -5150,7 +5169,7 @@
       </c>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>326</v>
       </c>
@@ -5188,7 +5207,7 @@
       </c>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>329</v>
       </c>
@@ -5226,7 +5245,7 @@
       </c>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>327</v>
       </c>
@@ -5264,7 +5283,7 @@
       </c>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>334</v>
       </c>
@@ -5302,7 +5321,7 @@
       </c>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>326</v>
       </c>
@@ -5340,7 +5359,7 @@
       </c>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>338</v>
       </c>
@@ -5378,7 +5397,7 @@
       </c>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>341</v>
       </c>
@@ -5416,7 +5435,7 @@
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>344</v>
       </c>
@@ -5454,7 +5473,7 @@
       </c>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>315</v>
       </c>
@@ -5492,7 +5511,7 @@
       </c>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>315</v>
       </c>
@@ -5530,7 +5549,7 @@
       </c>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>310</v>
       </c>
@@ -5568,7 +5587,7 @@
       </c>
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>322</v>
       </c>
@@ -5606,7 +5625,7 @@
       </c>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -5644,7 +5663,7 @@
       </c>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>355</v>
       </c>
@@ -5682,7 +5701,7 @@
       </c>
       <c r="N26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>358</v>
       </c>
@@ -5720,7 +5739,7 @@
       </c>
       <c r="N27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>360</v>
       </c>
@@ -5758,7 +5777,7 @@
       </c>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>360</v>
       </c>
@@ -5796,7 +5815,7 @@
       </c>
       <c r="N29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>364</v>
       </c>
@@ -5834,7 +5853,7 @@
       </c>
       <c r="N30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>367</v>
       </c>
@@ -5872,7 +5891,7 @@
       </c>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>304</v>
       </c>
@@ -5910,7 +5929,7 @@
       </c>
       <c r="N32" s="4"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>371</v>
       </c>
@@ -5948,11 +5967,51 @@
       </c>
       <c r="N33" s="4"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D34" s="4"/>
-      <c r="N34" s="4"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D34" s="2">
+        <v>20982</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CRUZJIMÉNEZVI@gmail.com</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J34" t="s">
+        <v>443</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO 'persona' VALUES ("VICTOR MANUEL","JIMÉNEZ","CRUZ",11/06/1957,"M","CRUZJIMÉNEZVI@gmail.com","9715765171","direccion de prueba","Juchitán","/directory/img-person/VICTORMANUELJIMENEZ.jpg"</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="F35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trabajando en datos para BD
</commit_message>
<xml_diff>
--- a/extras/datos/Lista Turorias 2019 luis.csv.xlsx
+++ b/extras/datos/Lista Turorias 2019 luis.csv.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tutorias\extras\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EECEEE-6E50-427F-AF79-39C14E7739B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="476">
   <si>
     <t>APELLIDO PATERNO</t>
   </si>
@@ -1444,13 +1451,22 @@
     <t>INSERT INTO 'persona' VALUES ("RANULFO","RIVERA","CASTILLO",25/09/1975,"M","CASTILLORIVERARA@gmail.com","9712325600","direccion de prueba","Unión Hidalgo","/directory/img-person/RANULFOCASTILLO.jpg"</t>
   </si>
   <si>
-    <t>d</t>
+    <t>JIMÉNEZ</t>
+  </si>
+  <si>
+    <t>VICTOR MANUEL</t>
+  </si>
+  <si>
+    <t>9715765171</t>
+  </si>
+  <si>
+    <t>/directory/img-person/VICTORMANUELJIMENEZ.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1541,7 +1557,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="2"/>
       <tableStyleElement type="headerRow" dxfId="1"/>
     </tableStyle>
@@ -1819,23 +1835,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView zoomScale="83" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1852,7 +1868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1869,7 +1885,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1886,7 +1902,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1903,7 +1919,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1920,7 +1936,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1937,7 +1953,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1954,7 +1970,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1971,7 +1987,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1988,7 +2004,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -2005,7 +2021,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2022,7 +2038,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -2039,7 +2055,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2056,7 +2072,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2073,7 +2089,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -2090,7 +2106,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2107,7 +2123,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2124,7 +2140,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2141,7 +2157,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2158,7 +2174,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2175,7 +2191,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -2192,7 +2208,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -2209,7 +2225,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -2226,7 +2242,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2243,7 +2259,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>55</v>
       </c>
@@ -2260,7 +2276,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -2277,7 +2293,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2294,7 +2310,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -2311,7 +2327,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -2328,7 +2344,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2345,7 +2361,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2362,7 +2378,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2379,7 +2395,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2396,7 +2412,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>75</v>
       </c>
@@ -2413,7 +2429,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>77</v>
       </c>
@@ -2430,7 +2446,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -2447,7 +2463,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -2464,7 +2480,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2481,7 +2497,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>91</v>
       </c>
@@ -2498,7 +2514,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>93</v>
       </c>
@@ -2515,7 +2531,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>95</v>
       </c>
@@ -2532,7 +2548,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>96</v>
       </c>
@@ -2549,7 +2565,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>105</v>
       </c>
@@ -2566,7 +2582,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>107</v>
       </c>
@@ -2583,7 +2599,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>108</v>
       </c>
@@ -2600,7 +2616,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>109</v>
       </c>
@@ -2617,7 +2633,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>111</v>
       </c>
@@ -2634,7 +2650,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -2651,7 +2667,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>114</v>
       </c>
@@ -2668,7 +2684,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -2685,7 +2701,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>19</v>
       </c>
@@ -2702,7 +2718,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>125</v>
       </c>
@@ -2719,7 +2735,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>127</v>
       </c>
@@ -2736,7 +2752,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>129</v>
       </c>
@@ -2753,7 +2769,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>129</v>
       </c>
@@ -2770,7 +2786,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>129</v>
       </c>
@@ -2787,7 +2803,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>132</v>
       </c>
@@ -2804,7 +2820,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -2821,7 +2837,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -2838,7 +2854,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -2855,7 +2871,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>32</v>
       </c>
@@ -2872,7 +2888,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>32</v>
       </c>
@@ -2889,7 +2905,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>145</v>
       </c>
@@ -2906,7 +2922,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>54</v>
       </c>
@@ -2923,7 +2939,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>146</v>
       </c>
@@ -2940,7 +2956,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -2957,7 +2973,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -2974,7 +2990,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>6</v>
       </c>
@@ -2991,7 +3007,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -3008,7 +3024,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -3025,7 +3041,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -3042,7 +3058,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>158</v>
       </c>
@@ -3059,7 +3075,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -3076,7 +3092,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>106</v>
       </c>
@@ -3093,7 +3109,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>160</v>
       </c>
@@ -3110,7 +3126,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>162</v>
       </c>
@@ -3127,7 +3143,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>95</v>
       </c>
@@ -3144,7 +3160,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>168</v>
       </c>
@@ -3161,7 +3177,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>170</v>
       </c>
@@ -3178,7 +3194,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -3195,7 +3211,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>172</v>
       </c>
@@ -3212,7 +3228,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>173</v>
       </c>
@@ -3229,7 +3245,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -3246,7 +3262,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>184</v>
       </c>
@@ -3263,7 +3279,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>186</v>
       </c>
@@ -3280,7 +3296,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>187</v>
       </c>
@@ -3297,7 +3313,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -3314,7 +3330,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>169</v>
       </c>
@@ -3331,7 +3347,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>189</v>
       </c>
@@ -3348,7 +3364,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>191</v>
       </c>
@@ -3365,7 +3381,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -3382,7 +3398,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>200</v>
       </c>
@@ -3399,7 +3415,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>26</v>
       </c>
@@ -3416,7 +3432,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>26</v>
       </c>
@@ -3433,7 +3449,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>145</v>
       </c>
@@ -3450,7 +3466,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>30</v>
       </c>
@@ -3467,7 +3483,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>30</v>
       </c>
@@ -3484,7 +3500,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>46</v>
       </c>
@@ -3501,7 +3517,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>46</v>
       </c>
@@ -3518,7 +3534,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>46</v>
       </c>
@@ -3535,7 +3551,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>162</v>
       </c>
@@ -3552,7 +3568,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>209</v>
       </c>
@@ -3569,7 +3585,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>208</v>
       </c>
@@ -3586,7 +3602,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>217</v>
       </c>
@@ -3603,7 +3619,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>5</v>
       </c>
@@ -3620,7 +3636,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>73</v>
       </c>
@@ -3637,7 +3653,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>219</v>
       </c>
@@ -3654,7 +3670,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>220</v>
       </c>
@@ -3671,7 +3687,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>222</v>
       </c>
@@ -3688,7 +3704,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>223</v>
       </c>
@@ -3714,32 +3730,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScale="82" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" customWidth="1"/>
-    <col min="10" max="10" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="30.5546875" customWidth="1"/>
+    <col min="10" max="10" width="56.109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="218" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="23.44140625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3771,7 +3787,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3818,7 +3834,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -3865,7 +3881,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -3905,7 +3921,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3945,7 +3961,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -3985,7 +4001,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -4025,7 +4041,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -4065,7 +4081,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -4105,7 +4121,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -4145,7 +4161,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -4182,7 +4198,7 @@
         <v>INSERT INTO 'persona' VALUES ("Jorge Antonio","Palomec","Lopez",08/11/1998,"M","LopezPalomecJo@gmail.com","9712152501","direccion prueba","Tehuantepec","/directory/img-person/JorgeAntonioPalomec.jpg"</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -4219,7 +4235,7 @@
         <v>INSERT INTO 'persona' VALUES ("Pedro Alberto","Perez","Martínez",14/03/1999,"M","MartínezPerezPe@gmail.com","9715094524","direccion prueba","Ixtepec","/directory/img-person/PedroAlbertoPerez.jpg"</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -4256,7 +4272,7 @@
         <v>INSERT INTO 'persona' VALUES ("Elías","Ramírez","Lugo",12/05/1999,"M","LugoRamírezEl@gmail.com","9716779058","direccion prueba","Juchitán","/directory/img-person/ElíasRamírez.jpg"</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -4293,7 +4309,7 @@
         <v>INSERT INTO 'persona' VALUES ("Sergio Manuel","Ramos","Jose",17/01/1999,"M","JoseRamosSe@gmail.com","9718404624","direccion prueba","Juchitán","/directory/img-person/SergioManuelRamos.jpg"</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -4330,7 +4346,7 @@
         <v>INSERT INTO 'persona' VALUES ("Carlos","Rasgado","López",18/08/1999,"M","LópezRasgadoCa@gmail.com","9718326392","direccion prueba","Chicapa","/directory/img-person/CarlosRasgado.jpg"</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -4367,7 +4383,7 @@
         <v>INSERT INTO 'persona' VALUES ("llliane Monserrat","Ruíz","Nuñez",20/09/1999,"F","NuñezRuízll@gmail.com","9713854313","direccion prueba","Salina Cruz","/directory/img-person/lllianeMonserratRuíz.jpg"</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -4404,7 +4420,7 @@
         <v>INSERT INTO 'persona' VALUES ("Arnulfo","Ruíz","Sánchez",17/06/1999,"M","SánchezRuízAr@gmail.com","9712820548","direccion prueba","Espinal","/directory/img-person/ArnulfoRuíz.jpg"</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -4441,7 +4457,7 @@
         <v>INSERT INTO 'persona' VALUES ("Esmeralda Yolotzin","Jiménez","Toledo",28/04/1999,"F","ToledoJiménezEs@gmail.com","9711441871","direccion prueba","Unión Hidalgo","/directory/img-person/EsmeraldaYolotzinJiménez.jpg"</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>53</v>
       </c>
@@ -4478,7 +4494,7 @@
         <v>INSERT INTO 'persona' VALUES ("Luis Alberto","Laureano","García",17/07/1999,"M","GarcíaLaureanoLu@gmail.com","9714388238","direccion prueba","Salina Cruz","/directory/img-person/LuisAlbertoLaureano.jpg"</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -4515,7 +4531,7 @@
         <v>INSERT INTO 'persona' VALUES ("Edwin","López","Hernandez",08/11/1997,"M","HernandezLópezEd@gmail.com","9715202809","direccion prueba","Unión Hidalgo","/directory/img-person/EdwinLópez.jpg"</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -4552,7 +4568,7 @@
         <v>INSERT INTO 'persona' VALUES ("Kevin","López","López",07/12/1999,"M","LópezLópezKe@gmail.com","9718406718","direccion prueba","Juchitán","/directory/img-person/KevinLópez.jpg"</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -4589,7 +4605,7 @@
         <v>INSERT INTO 'persona' VALUES ("Rey David","López","López",02/11/1999,"M","LópezLópezRe@gmail.com","9715018270","direccion prueba","Ixtepec","/directory/img-person/ReyDavidLópez.jpg"</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -4626,7 +4642,7 @@
         <v>INSERT INTO 'persona' VALUES ("Vladimir Orion","López","Matus",13/08/1997,"M","MatusLópezVl@gmail.com","9712271009","direccion prueba","Unión Hidalgo","/directory/img-person/VladimirOrionLópez.jpg"</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
@@ -4663,7 +4679,7 @@
         <v>INSERT INTO 'persona' VALUES ("Patricia Dhamar","Martínez","Chicaty",25/07/1999,"F","ChicatyMartínezPa@gmail.com","9719884435","direccion prueba","Ixtaltepec","/directory/img-person/PatriciaDhamarMartínez.jpg"</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -4700,7 +4716,7 @@
         <v>INSERT INTO 'persona' VALUES ("Guadalupe","Matus","Martínez",16/03/1998,"F","MartínezMatusGu@gmail.com","9714017985","direccion prueba","Espinal","/directory/img-person/GuadalupeMatus.jpg"</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -4743,33 +4759,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" customWidth="1"/>
-    <col min="7" max="7" width="31.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="51.85546875" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="196.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
+    <col min="10" max="10" width="51.88671875" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="12" max="12" width="196.33203125" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="19" max="19" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="19" max="19" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4801,7 +4817,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>298</v>
       </c>
@@ -4841,13 +4857,13 @@
       </c>
       <c r="Q2">
         <f>COUNTIF(E:E,"M")</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>301</v>
       </c>
@@ -4864,7 +4880,7 @@
         <v>234</v>
       </c>
       <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F33" si="0">CONCATENATE(B3,A3,LEFT(C3,2),"@gmail.com")</f>
+        <f t="shared" ref="F3:F34" si="0">CONCATENATE(B3,A3,LEFT(C3,2),"@gmail.com")</f>
         <v>GONZALEZPERALTALO@gmail.com</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -4893,7 +4909,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>304</v>
       </c>
@@ -4932,7 +4948,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>307</v>
       </c>
@@ -4971,7 +4987,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>310</v>
       </c>
@@ -5010,7 +5026,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>310</v>
       </c>
@@ -5049,7 +5065,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>315</v>
       </c>
@@ -5088,7 +5104,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>317</v>
       </c>
@@ -5123,14 +5139,11 @@
       <c r="L9" t="s">
         <v>447</v>
       </c>
-      <c r="P9" t="s">
-        <v>472</v>
-      </c>
       <c r="S9" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>315</v>
       </c>
@@ -5167,7 +5180,7 @@
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>322</v>
       </c>
@@ -5204,7 +5217,7 @@
       </c>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>315</v>
       </c>
@@ -5241,7 +5254,7 @@
       </c>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>326</v>
       </c>
@@ -5278,7 +5291,7 @@
       </c>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>329</v>
       </c>
@@ -5315,7 +5328,7 @@
       </c>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>327</v>
       </c>
@@ -5352,7 +5365,7 @@
       </c>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>334</v>
       </c>
@@ -5389,7 +5402,7 @@
       </c>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>326</v>
       </c>
@@ -5426,7 +5439,7 @@
       </c>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>338</v>
       </c>
@@ -5463,7 +5476,7 @@
       </c>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>341</v>
       </c>
@@ -5500,7 +5513,7 @@
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>344</v>
       </c>
@@ -5537,7 +5550,7 @@
       </c>
       <c r="N20" s="4"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>315</v>
       </c>
@@ -5574,7 +5587,7 @@
       </c>
       <c r="N21" s="4"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>315</v>
       </c>
@@ -5611,7 +5624,7 @@
       </c>
       <c r="N22" s="4"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>310</v>
       </c>
@@ -5648,7 +5661,7 @@
       </c>
       <c r="N23" s="4"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>322</v>
       </c>
@@ -5685,7 +5698,7 @@
       </c>
       <c r="N24" s="4"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>317</v>
       </c>
@@ -5722,7 +5735,7 @@
       </c>
       <c r="N25" s="4"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>355</v>
       </c>
@@ -5759,7 +5772,7 @@
       </c>
       <c r="N26" s="4"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>358</v>
       </c>
@@ -5796,7 +5809,7 @@
       </c>
       <c r="N27" s="4"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>360</v>
       </c>
@@ -5833,7 +5846,7 @@
       </c>
       <c r="N28" s="4"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>360</v>
       </c>
@@ -5870,7 +5883,7 @@
       </c>
       <c r="N29" s="4"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>364</v>
       </c>
@@ -5907,7 +5920,7 @@
       </c>
       <c r="N30" s="4"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>367</v>
       </c>
@@ -5944,7 +5957,7 @@
       </c>
       <c r="N31" s="4"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>304</v>
       </c>
@@ -5981,7 +5994,7 @@
       </c>
       <c r="N32" s="4"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>371</v>
       </c>
@@ -6018,8 +6031,42 @@
       </c>
       <c r="N33" s="4"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D34" s="4"/>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D34" s="2">
+        <v>20982</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>CRUZJIMÉNEZVI@gmail.com</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="J34" t="s">
+        <v>475</v>
+      </c>
+      <c r="L34" t="str">
+        <f t="shared" ref="L34" si="1">CONCATENATE("INSERT INTO 'persona' VALUES (",$S$2,C34,$S$2,",",$S$2,A34,$S$2,",",$S$2,B34,$S$2,",",TEXT(D34,"dd/mm/aaaa"),",",$S$2,E34,$S$2,",",$S$2,F34,$S$2,",",$S$2,G34,$S$2,",",$S$2,H34,$S$2,",",$S$2,I34,$S$2,",",$S$2,J34,$S$2)</f>
+        <v>INSERT INTO 'persona' VALUES ("VICTOR MANUEL","JIMÉNEZ","CRUZ",11/06/1957,"M","CRUZJIMÉNEZVI@gmail.com","9715765171","direccion de prueba","Juchitán","/directory/img-person/VICTORMANUELJIMENEZ.jpg"</v>
+      </c>
       <c r="N34" s="4"/>
     </row>
   </sheetData>

</xml_diff>